<commit_message>
Updated Seitzman 300 ROIs
Updated outer sphere radius for Seitzman 300 ROIs
</commit_message>
<xml_diff>
--- a/atlases/01_Seitzman 300_ROIs/Seitzman_300ROIs.xlsx
+++ b/atlases/01_Seitzman 300_ROIs/Seitzman_300ROIs.xlsx
@@ -1433,7 +1433,7 @@
   <dimension ref="A1:H301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection sqref="A1:H301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,7 +1487,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -1539,7 +1539,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -1565,7 +1565,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -1591,7 +1591,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -1617,7 +1617,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -1643,7 +1643,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -1669,7 +1669,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -1695,7 +1695,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -1721,7 +1721,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -1747,7 +1747,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -1773,7 +1773,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -1799,7 +1799,7 @@
         <v>5</v>
       </c>
       <c r="F14" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G14">
         <v>10</v>
@@ -1825,7 +1825,7 @@
         <v>5</v>
       </c>
       <c r="F15" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G15">
         <v>10</v>
@@ -1851,7 +1851,7 @@
         <v>5</v>
       </c>
       <c r="F16" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>10</v>
@@ -1877,7 +1877,7 @@
         <v>5</v>
       </c>
       <c r="F17" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G17">
         <v>10</v>
@@ -1903,7 +1903,7 @@
         <v>5</v>
       </c>
       <c r="F18" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G18">
         <v>10</v>
@@ -1929,7 +1929,7 @@
         <v>5</v>
       </c>
       <c r="F19" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G19">
         <v>10</v>
@@ -1955,7 +1955,7 @@
         <v>5</v>
       </c>
       <c r="F20" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G20">
         <v>10</v>
@@ -1981,7 +1981,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G21">
         <v>10</v>
@@ -2007,7 +2007,7 @@
         <v>5</v>
       </c>
       <c r="F22" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G22">
         <v>10</v>
@@ -2033,7 +2033,7 @@
         <v>5</v>
       </c>
       <c r="F23" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G23">
         <v>10</v>
@@ -2059,7 +2059,7 @@
         <v>5</v>
       </c>
       <c r="F24" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G24">
         <v>10</v>
@@ -2085,7 +2085,7 @@
         <v>5</v>
       </c>
       <c r="F25" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G25">
         <v>10</v>
@@ -2111,7 +2111,7 @@
         <v>5</v>
       </c>
       <c r="F26" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G26">
         <v>10</v>
@@ -2137,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="F27" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G27">
         <v>10</v>
@@ -2163,7 +2163,7 @@
         <v>5</v>
       </c>
       <c r="F28" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G28">
         <v>10</v>
@@ -2189,7 +2189,7 @@
         <v>5</v>
       </c>
       <c r="F29" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G29">
         <v>10</v>
@@ -2215,7 +2215,7 @@
         <v>5</v>
       </c>
       <c r="F30" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G30">
         <v>10</v>
@@ -2241,7 +2241,7 @@
         <v>5</v>
       </c>
       <c r="F31" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G31">
         <v>10</v>
@@ -2267,7 +2267,7 @@
         <v>5</v>
       </c>
       <c r="F32" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G32">
         <v>10</v>
@@ -2293,7 +2293,7 @@
         <v>5</v>
       </c>
       <c r="F33" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G33">
         <v>10</v>
@@ -2319,7 +2319,7 @@
         <v>5</v>
       </c>
       <c r="F34" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G34">
         <v>10</v>
@@ -2345,7 +2345,7 @@
         <v>5</v>
       </c>
       <c r="F35" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G35">
         <v>10</v>
@@ -2371,7 +2371,7 @@
         <v>5</v>
       </c>
       <c r="F36" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G36">
         <v>10</v>
@@ -2397,7 +2397,7 @@
         <v>5</v>
       </c>
       <c r="F37" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G37">
         <v>10</v>
@@ -2423,7 +2423,7 @@
         <v>5</v>
       </c>
       <c r="F38" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G38">
         <v>10</v>
@@ -2449,7 +2449,7 @@
         <v>5</v>
       </c>
       <c r="F39" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G39">
         <v>10</v>
@@ -2475,7 +2475,7 @@
         <v>5</v>
       </c>
       <c r="F40" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G40">
         <v>10</v>
@@ -2501,7 +2501,7 @@
         <v>5</v>
       </c>
       <c r="F41" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G41">
         <v>10</v>
@@ -2527,7 +2527,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G42">
         <v>10</v>
@@ -2553,7 +2553,7 @@
         <v>5</v>
       </c>
       <c r="F43" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G43">
         <v>10</v>
@@ -2579,7 +2579,7 @@
         <v>5</v>
       </c>
       <c r="F44" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G44">
         <v>10</v>
@@ -2605,7 +2605,7 @@
         <v>5</v>
       </c>
       <c r="F45" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G45">
         <v>10</v>
@@ -2631,7 +2631,7 @@
         <v>5</v>
       </c>
       <c r="F46" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G46">
         <v>11</v>
@@ -2657,7 +2657,7 @@
         <v>5</v>
       </c>
       <c r="F47" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G47">
         <v>11</v>
@@ -2683,7 +2683,7 @@
         <v>5</v>
       </c>
       <c r="F48" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G48">
         <v>11</v>
@@ -2709,7 +2709,7 @@
         <v>5</v>
       </c>
       <c r="F49" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G49">
         <v>11</v>
@@ -2735,7 +2735,7 @@
         <v>5</v>
       </c>
       <c r="F50" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G50">
         <v>11</v>
@@ -2761,7 +2761,7 @@
         <v>5</v>
       </c>
       <c r="F51" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G51">
         <v>9</v>
@@ -2787,7 +2787,7 @@
         <v>5</v>
       </c>
       <c r="F52" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G52">
         <v>9</v>
@@ -2813,7 +2813,7 @@
         <v>5</v>
       </c>
       <c r="F53" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G53">
         <v>9</v>
@@ -2839,7 +2839,7 @@
         <v>5</v>
       </c>
       <c r="F54" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G54">
         <v>9</v>
@@ -2865,7 +2865,7 @@
         <v>5</v>
       </c>
       <c r="F55" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G55">
         <v>9</v>
@@ -2891,7 +2891,7 @@
         <v>5</v>
       </c>
       <c r="F56" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G56">
         <v>9</v>
@@ -2917,7 +2917,7 @@
         <v>5</v>
       </c>
       <c r="F57" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G57">
         <v>9</v>
@@ -2943,7 +2943,7 @@
         <v>5</v>
       </c>
       <c r="F58" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G58">
         <v>9</v>
@@ -2969,7 +2969,7 @@
         <v>5</v>
       </c>
       <c r="F59" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G59">
         <v>9</v>
@@ -2995,7 +2995,7 @@
         <v>5</v>
       </c>
       <c r="F60" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G60">
         <v>9</v>
@@ -3021,7 +3021,7 @@
         <v>5</v>
       </c>
       <c r="F61" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G61">
         <v>9</v>
@@ -3047,7 +3047,7 @@
         <v>5</v>
       </c>
       <c r="F62" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G62">
         <v>9</v>
@@ -3073,7 +3073,7 @@
         <v>5</v>
       </c>
       <c r="F63" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G63">
         <v>9</v>
@@ -3099,7 +3099,7 @@
         <v>5</v>
       </c>
       <c r="F64" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G64">
         <v>9</v>
@@ -3125,7 +3125,7 @@
         <v>5</v>
       </c>
       <c r="F65" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G65">
         <v>9</v>
@@ -3151,7 +3151,7 @@
         <v>5</v>
       </c>
       <c r="F66" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G66">
         <v>9</v>
@@ -3177,7 +3177,7 @@
         <v>5</v>
       </c>
       <c r="F67" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G67">
         <v>9</v>
@@ -3203,7 +3203,7 @@
         <v>5</v>
       </c>
       <c r="F68" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G68">
         <v>9</v>
@@ -3229,7 +3229,7 @@
         <v>5</v>
       </c>
       <c r="F69" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G69">
         <v>9</v>
@@ -3255,7 +3255,7 @@
         <v>5</v>
       </c>
       <c r="F70" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G70">
         <v>12</v>
@@ -3281,7 +3281,7 @@
         <v>5</v>
       </c>
       <c r="F71" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G71">
         <v>12</v>
@@ -3307,7 +3307,7 @@
         <v>5</v>
       </c>
       <c r="F72" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G72">
         <v>12</v>
@@ -3333,7 +3333,7 @@
         <v>5</v>
       </c>
       <c r="F73" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G73">
         <v>12</v>
@@ -3359,7 +3359,7 @@
         <v>5</v>
       </c>
       <c r="F74" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G74">
         <v>12</v>
@@ -3385,7 +3385,7 @@
         <v>5</v>
       </c>
       <c r="F75" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G75">
         <v>12</v>
@@ -3411,7 +3411,7 @@
         <v>5</v>
       </c>
       <c r="F76" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G76">
         <v>12</v>
@@ -3437,7 +3437,7 @@
         <v>5</v>
       </c>
       <c r="F77" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G77">
         <v>12</v>
@@ -3463,7 +3463,7 @@
         <v>5</v>
       </c>
       <c r="F78" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G78">
         <v>12</v>
@@ -3489,7 +3489,7 @@
         <v>5</v>
       </c>
       <c r="F79" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G79">
         <v>12</v>
@@ -3515,7 +3515,7 @@
         <v>5</v>
       </c>
       <c r="F80" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G80">
         <v>12</v>
@@ -3541,7 +3541,7 @@
         <v>5</v>
       </c>
       <c r="F81" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G81">
         <v>12</v>
@@ -3567,7 +3567,7 @@
         <v>5</v>
       </c>
       <c r="F82" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G82">
         <v>1</v>
@@ -3593,7 +3593,7 @@
         <v>5</v>
       </c>
       <c r="F83" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G83">
         <v>1</v>
@@ -3619,7 +3619,7 @@
         <v>5</v>
       </c>
       <c r="F84" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G84">
         <v>1</v>
@@ -3645,7 +3645,7 @@
         <v>5</v>
       </c>
       <c r="F85" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G85">
         <v>1</v>
@@ -3671,7 +3671,7 @@
         <v>5</v>
       </c>
       <c r="F86" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G86">
         <v>1</v>
@@ -3697,7 +3697,7 @@
         <v>5</v>
       </c>
       <c r="F87" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G87">
         <v>1</v>
@@ -3723,7 +3723,7 @@
         <v>5</v>
       </c>
       <c r="F88" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G88">
         <v>1</v>
@@ -3749,7 +3749,7 @@
         <v>5</v>
       </c>
       <c r="F89" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G89">
         <v>1</v>
@@ -3775,7 +3775,7 @@
         <v>5</v>
       </c>
       <c r="F90" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G90">
         <v>1</v>
@@ -3801,7 +3801,7 @@
         <v>5</v>
       </c>
       <c r="F91" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G91">
         <v>1</v>
@@ -3827,7 +3827,7 @@
         <v>5</v>
       </c>
       <c r="F92" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G92">
         <v>1</v>
@@ -3853,7 +3853,7 @@
         <v>5</v>
       </c>
       <c r="F93" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G93">
         <v>1</v>
@@ -3879,7 +3879,7 @@
         <v>5</v>
       </c>
       <c r="F94" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G94">
         <v>1</v>
@@ -3905,7 +3905,7 @@
         <v>5</v>
       </c>
       <c r="F95" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G95">
         <v>1</v>
@@ -3931,7 +3931,7 @@
         <v>5</v>
       </c>
       <c r="F96" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G96">
         <v>1</v>
@@ -3957,7 +3957,7 @@
         <v>5</v>
       </c>
       <c r="F97" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G97">
         <v>1</v>
@@ -3983,7 +3983,7 @@
         <v>5</v>
       </c>
       <c r="F98" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G98">
         <v>1</v>
@@ -4009,7 +4009,7 @@
         <v>5</v>
       </c>
       <c r="F99" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G99">
         <v>1</v>
@@ -4035,7 +4035,7 @@
         <v>5</v>
       </c>
       <c r="F100" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G100">
         <v>1</v>
@@ -4061,7 +4061,7 @@
         <v>5</v>
       </c>
       <c r="F101" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G101">
         <v>1</v>
@@ -4087,7 +4087,7 @@
         <v>5</v>
       </c>
       <c r="F102" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G102">
         <v>1</v>
@@ -4113,7 +4113,7 @@
         <v>5</v>
       </c>
       <c r="F103" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G103">
         <v>1</v>
@@ -4139,7 +4139,7 @@
         <v>5</v>
       </c>
       <c r="F104" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G104">
         <v>1</v>
@@ -4165,7 +4165,7 @@
         <v>5</v>
       </c>
       <c r="F105" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G105">
         <v>1</v>
@@ -4191,7 +4191,7 @@
         <v>5</v>
       </c>
       <c r="F106" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G106">
         <v>1</v>
@@ -4217,7 +4217,7 @@
         <v>5</v>
       </c>
       <c r="F107" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G107">
         <v>1</v>
@@ -4243,7 +4243,7 @@
         <v>5</v>
       </c>
       <c r="F108" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G108">
         <v>1</v>
@@ -4269,7 +4269,7 @@
         <v>5</v>
       </c>
       <c r="F109" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G109">
         <v>1</v>
@@ -4295,7 +4295,7 @@
         <v>5</v>
       </c>
       <c r="F110" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G110">
         <v>1</v>
@@ -4321,7 +4321,7 @@
         <v>5</v>
       </c>
       <c r="F111" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G111">
         <v>1</v>
@@ -4347,7 +4347,7 @@
         <v>5</v>
       </c>
       <c r="F112" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G112">
         <v>1</v>
@@ -4373,7 +4373,7 @@
         <v>5</v>
       </c>
       <c r="F113" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G113">
         <v>1</v>
@@ -4399,7 +4399,7 @@
         <v>5</v>
       </c>
       <c r="F114" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G114">
         <v>1</v>
@@ -4425,7 +4425,7 @@
         <v>5</v>
       </c>
       <c r="F115" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G115">
         <v>1</v>
@@ -4451,7 +4451,7 @@
         <v>5</v>
       </c>
       <c r="F116" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G116">
         <v>1</v>
@@ -4477,7 +4477,7 @@
         <v>5</v>
       </c>
       <c r="F117" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G117">
         <v>1</v>
@@ -4503,7 +4503,7 @@
         <v>5</v>
       </c>
       <c r="F118" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G118">
         <v>1</v>
@@ -4529,7 +4529,7 @@
         <v>5</v>
       </c>
       <c r="F119" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G119">
         <v>1</v>
@@ -4555,7 +4555,7 @@
         <v>5</v>
       </c>
       <c r="F120" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G120">
         <v>1</v>
@@ -4581,7 +4581,7 @@
         <v>5</v>
       </c>
       <c r="F121" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G121">
         <v>1</v>
@@ -4607,7 +4607,7 @@
         <v>5</v>
       </c>
       <c r="F122" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G122">
         <v>1</v>
@@ -4633,7 +4633,7 @@
         <v>5</v>
       </c>
       <c r="F123" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G123">
         <v>1</v>
@@ -4659,7 +4659,7 @@
         <v>5</v>
       </c>
       <c r="F124" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G124">
         <v>1</v>
@@ -4685,7 +4685,7 @@
         <v>5</v>
       </c>
       <c r="F125" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G125">
         <v>1</v>
@@ -4711,7 +4711,7 @@
         <v>5</v>
       </c>
       <c r="F126" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G126">
         <v>1</v>
@@ -4737,7 +4737,7 @@
         <v>5</v>
       </c>
       <c r="F127" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G127">
         <v>1</v>
@@ -4763,7 +4763,7 @@
         <v>5</v>
       </c>
       <c r="F128" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G128">
         <v>1</v>
@@ -4789,7 +4789,7 @@
         <v>5</v>
       </c>
       <c r="F129" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G129">
         <v>1</v>
@@ -4815,7 +4815,7 @@
         <v>5</v>
       </c>
       <c r="F130" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G130">
         <v>1</v>
@@ -4841,7 +4841,7 @@
         <v>5</v>
       </c>
       <c r="F131" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G131">
         <v>1</v>
@@ -4867,7 +4867,7 @@
         <v>5</v>
       </c>
       <c r="F132" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G132">
         <v>1</v>
@@ -4893,7 +4893,7 @@
         <v>5</v>
       </c>
       <c r="F133" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G133">
         <v>1</v>
@@ -4919,7 +4919,7 @@
         <v>5</v>
       </c>
       <c r="F134" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G134">
         <v>1</v>
@@ -4945,7 +4945,7 @@
         <v>5</v>
       </c>
       <c r="F135" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G135">
         <v>1</v>
@@ -4971,7 +4971,7 @@
         <v>5</v>
       </c>
       <c r="F136" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G136">
         <v>1</v>
@@ -4997,7 +4997,7 @@
         <v>5</v>
       </c>
       <c r="F137" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G137">
         <v>15</v>
@@ -5023,7 +5023,7 @@
         <v>5</v>
       </c>
       <c r="F138" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G138">
         <v>15</v>
@@ -5049,7 +5049,7 @@
         <v>5</v>
       </c>
       <c r="F139" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G139">
         <v>15</v>
@@ -5075,7 +5075,7 @@
         <v>5</v>
       </c>
       <c r="F140" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G140">
         <v>15</v>
@@ -5101,7 +5101,7 @@
         <v>5</v>
       </c>
       <c r="F141" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G141">
         <v>15</v>
@@ -5127,7 +5127,7 @@
         <v>5</v>
       </c>
       <c r="F142" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G142">
         <v>2</v>
@@ -5153,7 +5153,7 @@
         <v>5</v>
       </c>
       <c r="F143" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G143">
         <v>2</v>
@@ -5179,7 +5179,7 @@
         <v>5</v>
       </c>
       <c r="F144" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G144">
         <v>2</v>
@@ -5205,7 +5205,7 @@
         <v>5</v>
       </c>
       <c r="F145" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G145">
         <v>2</v>
@@ -5231,7 +5231,7 @@
         <v>5</v>
       </c>
       <c r="F146" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G146">
         <v>2</v>
@@ -5257,7 +5257,7 @@
         <v>5</v>
       </c>
       <c r="F147" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G147">
         <v>2</v>
@@ -5283,7 +5283,7 @@
         <v>5</v>
       </c>
       <c r="F148" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G148">
         <v>2</v>
@@ -5309,7 +5309,7 @@
         <v>5</v>
       </c>
       <c r="F149" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G149">
         <v>2</v>
@@ -5335,7 +5335,7 @@
         <v>5</v>
       </c>
       <c r="F150" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G150">
         <v>2</v>
@@ -5361,7 +5361,7 @@
         <v>5</v>
       </c>
       <c r="F151" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G151">
         <v>2</v>
@@ -5387,7 +5387,7 @@
         <v>5</v>
       </c>
       <c r="F152" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G152">
         <v>2</v>
@@ -5413,7 +5413,7 @@
         <v>5</v>
       </c>
       <c r="F153" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G153">
         <v>2</v>
@@ -5439,7 +5439,7 @@
         <v>5</v>
       </c>
       <c r="F154" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G154">
         <v>2</v>
@@ -5465,7 +5465,7 @@
         <v>5</v>
       </c>
       <c r="F155" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G155">
         <v>2</v>
@@ -5491,7 +5491,7 @@
         <v>5</v>
       </c>
       <c r="F156" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G156">
         <v>2</v>
@@ -5517,7 +5517,7 @@
         <v>5</v>
       </c>
       <c r="F157" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G157">
         <v>2</v>
@@ -5543,7 +5543,7 @@
         <v>5</v>
       </c>
       <c r="F158" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G158">
         <v>2</v>
@@ -5569,7 +5569,7 @@
         <v>5</v>
       </c>
       <c r="F159" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G159">
         <v>2</v>
@@ -5595,7 +5595,7 @@
         <v>5</v>
       </c>
       <c r="F160" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G160">
         <v>2</v>
@@ -5621,7 +5621,7 @@
         <v>5</v>
       </c>
       <c r="F161" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G161">
         <v>2</v>
@@ -5647,7 +5647,7 @@
         <v>5</v>
       </c>
       <c r="F162" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G162">
         <v>2</v>
@@ -5673,7 +5673,7 @@
         <v>5</v>
       </c>
       <c r="F163" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G163">
         <v>2</v>
@@ -5699,7 +5699,7 @@
         <v>5</v>
       </c>
       <c r="F164" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G164">
         <v>2</v>
@@ -5725,7 +5725,7 @@
         <v>5</v>
       </c>
       <c r="F165" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G165">
         <v>2</v>
@@ -5751,7 +5751,7 @@
         <v>5</v>
       </c>
       <c r="F166" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G166">
         <v>2</v>
@@ -5777,7 +5777,7 @@
         <v>5</v>
       </c>
       <c r="F167" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G167">
         <v>2</v>
@@ -5803,7 +5803,7 @@
         <v>5</v>
       </c>
       <c r="F168" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G168">
         <v>2</v>
@@ -5829,7 +5829,7 @@
         <v>5</v>
       </c>
       <c r="F169" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G169">
         <v>2</v>
@@ -5855,7 +5855,7 @@
         <v>5</v>
       </c>
       <c r="F170" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G170">
         <v>2</v>
@@ -5881,7 +5881,7 @@
         <v>5</v>
       </c>
       <c r="F171" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G171">
         <v>2</v>
@@ -5907,7 +5907,7 @@
         <v>5</v>
       </c>
       <c r="F172" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G172">
         <v>2</v>
@@ -5933,7 +5933,7 @@
         <v>5</v>
       </c>
       <c r="F173" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G173">
         <v>2</v>
@@ -5959,7 +5959,7 @@
         <v>5</v>
       </c>
       <c r="F174" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G174">
         <v>2</v>
@@ -5985,7 +5985,7 @@
         <v>5</v>
       </c>
       <c r="F175" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G175">
         <v>2</v>
@@ -6011,7 +6011,7 @@
         <v>5</v>
       </c>
       <c r="F176" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G176">
         <v>3</v>
@@ -6037,7 +6037,7 @@
         <v>5</v>
       </c>
       <c r="F177" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G177">
         <v>3</v>
@@ -6063,7 +6063,7 @@
         <v>5</v>
       </c>
       <c r="F178" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G178">
         <v>3</v>
@@ -6089,7 +6089,7 @@
         <v>5</v>
       </c>
       <c r="F179" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G179">
         <v>3</v>
@@ -6115,7 +6115,7 @@
         <v>5</v>
       </c>
       <c r="F180" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G180">
         <v>3</v>
@@ -6141,7 +6141,7 @@
         <v>5</v>
       </c>
       <c r="F181" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G181">
         <v>3</v>
@@ -6167,7 +6167,7 @@
         <v>5</v>
       </c>
       <c r="F182" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G182">
         <v>3</v>
@@ -6193,7 +6193,7 @@
         <v>5</v>
       </c>
       <c r="F183" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G183">
         <v>3</v>
@@ -6219,7 +6219,7 @@
         <v>5</v>
       </c>
       <c r="F184" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G184">
         <v>3</v>
@@ -6245,7 +6245,7 @@
         <v>5</v>
       </c>
       <c r="F185" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G185">
         <v>3</v>
@@ -6271,7 +6271,7 @@
         <v>5</v>
       </c>
       <c r="F186" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G186">
         <v>3</v>
@@ -6297,7 +6297,7 @@
         <v>5</v>
       </c>
       <c r="F187" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G187">
         <v>3</v>
@@ -6323,7 +6323,7 @@
         <v>5</v>
       </c>
       <c r="F188" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G188">
         <v>3</v>
@@ -6349,7 +6349,7 @@
         <v>5</v>
       </c>
       <c r="F189" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G189">
         <v>3</v>
@@ -6375,7 +6375,7 @@
         <v>5</v>
       </c>
       <c r="F190" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G190">
         <v>3</v>
@@ -6401,7 +6401,7 @@
         <v>5</v>
       </c>
       <c r="F191" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G191">
         <v>3</v>
@@ -6427,7 +6427,7 @@
         <v>5</v>
       </c>
       <c r="F192" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G192">
         <v>3</v>
@@ -6453,7 +6453,7 @@
         <v>5</v>
       </c>
       <c r="F193" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G193">
         <v>3</v>
@@ -6479,7 +6479,7 @@
         <v>5</v>
       </c>
       <c r="F194" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G194">
         <v>3</v>
@@ -6505,7 +6505,7 @@
         <v>5</v>
       </c>
       <c r="F195" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G195">
         <v>3</v>
@@ -6531,7 +6531,7 @@
         <v>5</v>
       </c>
       <c r="F196" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G196">
         <v>3</v>
@@ -6557,7 +6557,7 @@
         <v>5</v>
       </c>
       <c r="F197" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G197">
         <v>3</v>
@@ -6583,7 +6583,7 @@
         <v>5</v>
       </c>
       <c r="F198" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G198">
         <v>3</v>
@@ -6609,7 +6609,7 @@
         <v>5</v>
       </c>
       <c r="F199" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G199">
         <v>3</v>
@@ -6635,7 +6635,7 @@
         <v>5</v>
       </c>
       <c r="F200" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G200">
         <v>3</v>
@@ -6661,7 +6661,7 @@
         <v>5</v>
       </c>
       <c r="F201" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G201">
         <v>3</v>
@@ -6687,7 +6687,7 @@
         <v>5</v>
       </c>
       <c r="F202" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G202">
         <v>3</v>
@@ -6713,7 +6713,7 @@
         <v>5</v>
       </c>
       <c r="F203" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G203">
         <v>8</v>
@@ -6739,7 +6739,7 @@
         <v>5</v>
       </c>
       <c r="F204" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G204">
         <v>8</v>
@@ -6765,7 +6765,7 @@
         <v>5</v>
       </c>
       <c r="F205" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G205">
         <v>8</v>
@@ -6791,7 +6791,7 @@
         <v>5</v>
       </c>
       <c r="F206" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G206">
         <v>8</v>
@@ -6817,7 +6817,7 @@
         <v>5</v>
       </c>
       <c r="F207" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G207">
         <v>8</v>
@@ -6843,7 +6843,7 @@
         <v>5</v>
       </c>
       <c r="F208" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G208">
         <v>8</v>
@@ -6869,7 +6869,7 @@
         <v>5</v>
       </c>
       <c r="F209" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G209">
         <v>8</v>
@@ -6895,7 +6895,7 @@
         <v>5</v>
       </c>
       <c r="F210" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G210">
         <v>8</v>
@@ -6921,7 +6921,7 @@
         <v>5</v>
       </c>
       <c r="F211" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G211">
         <v>8</v>
@@ -6947,7 +6947,7 @@
         <v>5</v>
       </c>
       <c r="F212" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G212">
         <v>7</v>
@@ -6973,7 +6973,7 @@
         <v>5</v>
       </c>
       <c r="F213" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G213">
         <v>7</v>
@@ -6999,7 +6999,7 @@
         <v>5</v>
       </c>
       <c r="F214" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G214">
         <v>7</v>
@@ -7025,7 +7025,7 @@
         <v>5</v>
       </c>
       <c r="F215" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G215">
         <v>7</v>
@@ -7051,7 +7051,7 @@
         <v>5</v>
       </c>
       <c r="F216" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G216">
         <v>7</v>
@@ -7077,7 +7077,7 @@
         <v>5</v>
       </c>
       <c r="F217" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G217">
         <v>7</v>
@@ -7103,7 +7103,7 @@
         <v>5</v>
       </c>
       <c r="F218" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G218">
         <v>7</v>
@@ -7129,7 +7129,7 @@
         <v>5</v>
       </c>
       <c r="F219" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G219">
         <v>7</v>
@@ -7155,7 +7155,7 @@
         <v>5</v>
       </c>
       <c r="F220" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G220">
         <v>7</v>
@@ -7181,7 +7181,7 @@
         <v>5</v>
       </c>
       <c r="F221" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G221">
         <v>5</v>
@@ -7207,7 +7207,7 @@
         <v>5</v>
       </c>
       <c r="F222" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G222">
         <v>5</v>
@@ -7233,7 +7233,7 @@
         <v>5</v>
       </c>
       <c r="F223" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G223">
         <v>5</v>
@@ -7259,7 +7259,7 @@
         <v>5</v>
       </c>
       <c r="F224" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G224">
         <v>5</v>
@@ -7285,7 +7285,7 @@
         <v>5</v>
       </c>
       <c r="F225" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G225">
         <v>5</v>
@@ -7311,7 +7311,7 @@
         <v>5</v>
       </c>
       <c r="F226" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G226">
         <v>5</v>
@@ -7337,7 +7337,7 @@
         <v>5</v>
       </c>
       <c r="F227" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G227">
         <v>5</v>
@@ -7363,7 +7363,7 @@
         <v>5</v>
       </c>
       <c r="F228" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G228">
         <v>5</v>
@@ -7389,7 +7389,7 @@
         <v>5</v>
       </c>
       <c r="F229" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G229">
         <v>5</v>
@@ -7415,7 +7415,7 @@
         <v>5</v>
       </c>
       <c r="F230" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G230">
         <v>5</v>
@@ -7441,7 +7441,7 @@
         <v>5</v>
       </c>
       <c r="F231" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G231">
         <v>5</v>
@@ -7467,7 +7467,7 @@
         <v>5</v>
       </c>
       <c r="F232" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G232">
         <v>5</v>
@@ -7493,7 +7493,7 @@
         <v>5</v>
       </c>
       <c r="F233" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G233">
         <v>5</v>
@@ -7519,7 +7519,7 @@
         <v>5</v>
       </c>
       <c r="F234" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G234">
         <v>5</v>
@@ -7545,7 +7545,7 @@
         <v>5</v>
       </c>
       <c r="F235" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G235">
         <v>17</v>
@@ -7571,7 +7571,7 @@
         <v>5</v>
       </c>
       <c r="F236" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G236">
         <v>17</v>
@@ -7597,7 +7597,7 @@
         <v>4</v>
       </c>
       <c r="F237">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G237">
         <v>17</v>
@@ -7623,7 +7623,7 @@
         <v>4</v>
       </c>
       <c r="F238">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G238">
         <v>17</v>
@@ -7649,7 +7649,7 @@
         <v>4</v>
       </c>
       <c r="F239">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G239">
         <v>1</v>
@@ -7675,7 +7675,7 @@
         <v>4</v>
       </c>
       <c r="F240">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G240">
         <v>1</v>
@@ -7701,7 +7701,7 @@
         <v>5</v>
       </c>
       <c r="F241" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G241">
         <v>4</v>
@@ -7727,7 +7727,7 @@
         <v>5</v>
       </c>
       <c r="F242" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G242">
         <v>4</v>
@@ -7753,7 +7753,7 @@
         <v>5</v>
       </c>
       <c r="F243" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G243">
         <v>4</v>
@@ -7779,7 +7779,7 @@
         <v>5</v>
       </c>
       <c r="F244" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G244">
         <v>4</v>
@@ -7805,7 +7805,7 @@
         <v>4</v>
       </c>
       <c r="F245">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G245">
         <v>4</v>
@@ -7831,7 +7831,7 @@
         <v>4</v>
       </c>
       <c r="F246">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G246">
         <v>4</v>
@@ -7857,7 +7857,7 @@
         <v>4</v>
       </c>
       <c r="F247">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G247">
         <v>4</v>
@@ -7883,7 +7883,7 @@
         <v>4</v>
       </c>
       <c r="F248">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G248">
         <v>4</v>
@@ -7909,7 +7909,7 @@
         <v>4</v>
       </c>
       <c r="F249">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G249">
         <v>1</v>
@@ -7935,7 +7935,7 @@
         <v>4</v>
       </c>
       <c r="F250">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G250">
         <v>1</v>
@@ -7961,7 +7961,7 @@
         <v>4</v>
       </c>
       <c r="F251">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G251">
         <v>3</v>
@@ -7987,7 +7987,7 @@
         <v>4</v>
       </c>
       <c r="F252">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G252">
         <v>3</v>
@@ -8013,7 +8013,7 @@
         <v>4</v>
       </c>
       <c r="F253">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G253">
         <v>10</v>
@@ -8039,7 +8039,7 @@
         <v>4</v>
       </c>
       <c r="F254">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G254">
         <v>10</v>
@@ -8065,7 +8065,7 @@
         <v>4</v>
       </c>
       <c r="F255">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G255">
         <v>10</v>
@@ -8091,7 +8091,7 @@
         <v>4</v>
       </c>
       <c r="F256">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G256">
         <v>10</v>
@@ -8117,7 +8117,7 @@
         <v>4</v>
       </c>
       <c r="F257">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G257">
         <v>10</v>
@@ -8143,7 +8143,7 @@
         <v>4</v>
       </c>
       <c r="F258">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G258">
         <v>10</v>
@@ -8169,7 +8169,7 @@
         <v>4</v>
       </c>
       <c r="F259">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G259">
         <v>10</v>
@@ -8195,7 +8195,7 @@
         <v>4</v>
       </c>
       <c r="F260">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G260">
         <v>10</v>
@@ -8221,7 +8221,7 @@
         <v>4</v>
       </c>
       <c r="F261">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G261">
         <v>10</v>
@@ -8247,7 +8247,7 @@
         <v>4</v>
       </c>
       <c r="F262">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G262">
         <v>10</v>
@@ -8273,7 +8273,7 @@
         <v>4</v>
       </c>
       <c r="F263">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G263">
         <v>1</v>
@@ -8299,7 +8299,7 @@
         <v>4</v>
       </c>
       <c r="F264">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G264">
         <v>1</v>
@@ -8325,7 +8325,7 @@
         <v>4</v>
       </c>
       <c r="F265">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G265">
         <v>2</v>
@@ -8351,7 +8351,7 @@
         <v>4</v>
       </c>
       <c r="F266">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G266">
         <v>2</v>
@@ -8377,7 +8377,7 @@
         <v>4</v>
       </c>
       <c r="F267">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G267">
         <v>9</v>
@@ -8403,7 +8403,7 @@
         <v>4</v>
       </c>
       <c r="F268">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G268">
         <v>9</v>
@@ -8429,7 +8429,7 @@
         <v>4</v>
       </c>
       <c r="F269">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G269">
         <v>9</v>
@@ -8455,7 +8455,7 @@
         <v>4</v>
       </c>
       <c r="F270">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G270">
         <v>9</v>
@@ -8481,7 +8481,7 @@
         <v>4</v>
       </c>
       <c r="F271">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G271">
         <v>10</v>
@@ -8507,7 +8507,7 @@
         <v>4</v>
       </c>
       <c r="F272">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G272">
         <v>10</v>
@@ -8533,7 +8533,7 @@
         <v>4</v>
       </c>
       <c r="F273">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G273">
         <v>10</v>
@@ -8559,7 +8559,7 @@
         <v>4</v>
       </c>
       <c r="F274">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G274">
         <v>10</v>
@@ -8585,7 +8585,7 @@
         <v>4</v>
       </c>
       <c r="F275">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G275" s="1">
         <v>0</v>
@@ -8611,7 +8611,7 @@
         <v>4</v>
       </c>
       <c r="F276">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G276" s="1">
         <v>0</v>
@@ -8637,7 +8637,7 @@
         <v>4</v>
       </c>
       <c r="F277">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G277" s="1">
         <v>0</v>
@@ -8663,7 +8663,7 @@
         <v>4</v>
       </c>
       <c r="F278">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G278">
         <v>1</v>
@@ -8689,7 +8689,7 @@
         <v>4</v>
       </c>
       <c r="F279">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G279">
         <v>1</v>
@@ -8715,7 +8715,7 @@
         <v>4</v>
       </c>
       <c r="F280">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G280">
         <v>1</v>
@@ -8741,7 +8741,7 @@
         <v>4</v>
       </c>
       <c r="F281">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G281">
         <v>1</v>
@@ -8767,7 +8767,7 @@
         <v>4</v>
       </c>
       <c r="F282">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G282">
         <v>1</v>
@@ -8793,7 +8793,7 @@
         <v>4</v>
       </c>
       <c r="F283">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G283">
         <v>1</v>
@@ -8819,7 +8819,7 @@
         <v>4</v>
       </c>
       <c r="F284">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G284">
         <v>2</v>
@@ -8845,7 +8845,7 @@
         <v>4</v>
       </c>
       <c r="F285">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G285">
         <v>3</v>
@@ -8871,7 +8871,7 @@
         <v>4</v>
       </c>
       <c r="F286">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G286">
         <v>3</v>
@@ -8897,7 +8897,7 @@
         <v>4</v>
       </c>
       <c r="F287">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G287">
         <v>3</v>
@@ -8923,7 +8923,7 @@
         <v>4</v>
       </c>
       <c r="F288">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G288">
         <v>3</v>
@@ -8949,7 +8949,7 @@
         <v>4</v>
       </c>
       <c r="F289">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G289">
         <v>3</v>
@@ -8975,7 +8975,7 @@
         <v>4</v>
       </c>
       <c r="F290">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G290">
         <v>3</v>
@@ -9001,7 +9001,7 @@
         <v>4</v>
       </c>
       <c r="F291">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G291">
         <v>3</v>
@@ -9027,7 +9027,7 @@
         <v>4</v>
       </c>
       <c r="F292">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G292">
         <v>9</v>
@@ -9053,7 +9053,7 @@
         <v>4</v>
       </c>
       <c r="F293">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G293">
         <v>9</v>
@@ -9079,7 +9079,7 @@
         <v>4</v>
       </c>
       <c r="F294">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G294">
         <v>9</v>
@@ -9105,7 +9105,7 @@
         <v>4</v>
       </c>
       <c r="F295">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G295">
         <v>10</v>
@@ -9131,7 +9131,7 @@
         <v>4</v>
       </c>
       <c r="F296">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G296">
         <v>10</v>
@@ -9157,7 +9157,7 @@
         <v>4</v>
       </c>
       <c r="F297">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G297">
         <v>10</v>
@@ -9183,7 +9183,7 @@
         <v>4</v>
       </c>
       <c r="F298">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G298">
         <v>10</v>
@@ -9209,7 +9209,7 @@
         <v>4</v>
       </c>
       <c r="F299">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G299">
         <v>10</v>
@@ -9235,7 +9235,7 @@
         <v>4</v>
       </c>
       <c r="F300">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G300">
         <v>10</v>
@@ -9261,7 +9261,7 @@
         <v>4</v>
       </c>
       <c r="F301">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G301">
         <v>10</v>

</xml_diff>